<commit_message>
added some israeli logic and confilct solution for importing guests
</commit_message>
<xml_diff>
--- a/resources/guest_list.xlsx
+++ b/resources/guest_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyma\Desktop\Projects\Wedding_web\wedding\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB0A30F-7CE6-4B57-92B1-7320B549FECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C27DFB-67F1-4783-887E-D7AA057C1058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="21336" windowHeight="11268" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guests" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>guy.gm.maduel@gmail.com</t>
+  </si>
+  <si>
+    <t>whatsapp</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>link</t>
   </si>
 </sst>
 </file>
@@ -416,15 +425,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="81.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,80 +467,103 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="I2" t="b">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>